<commit_message>
SSDM-13256: Excluded "$" and "Auto generate codes" from the list of default attributes when exporting samples not for import.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t xml:space="preserve">SAMPLE</t>
   </si>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">DEFAULT</t>
   </si>
   <si>
-    <t xml:space="preserve">$</t>
-  </si>
-  <si>
     <t xml:space="preserve">Identifier</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t xml:space="preserve">Experiment</t>
   </si>
   <si>
-    <t xml:space="preserve">Auto generate codes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parents</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">/DEFAULT/DEFAULT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">system</t>
@@ -160,10 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -278,7 +268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,10 +309,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -331,7 +317,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,10 +342,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD14"/>
+  <dimension ref="A1:AMM14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10:G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -369,14 +355,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="26.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1027" min="1027" style="1" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1026" min="1026" style="1" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="8.37"/>
   </cols>
   <sheetData>
@@ -408,7 +394,7 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -417,16 +403,16 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -435,70 +421,57 @@
       <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="AMK4" s="1"/>
+      <c r="AMM4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="AMM4" s="0"/>
-      <c r="AMN4" s="1"/>
-      <c r="AMO4" s="1"/>
-      <c r="XFD4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AMM5" s="0"/>
-      <c r="AMN5" s="1"/>
-      <c r="AMO5" s="1"/>
-      <c r="XFD5" s="0"/>
+      <c r="AMK5" s="1"/>
+      <c r="AMM5" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -511,7 +484,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -522,7 +495,7 @@
       <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -531,16 +504,16 @@
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -549,210 +522,178 @@
       <c r="K10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="9" t="s">
+      <c r="M10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="AMK10" s="1"/>
+      <c r="AMM10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="AMM10" s="0"/>
-      <c r="AMN10" s="1"/>
-      <c r="AMO10" s="1"/>
-      <c r="XFD10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="M11" s="10" t="n">
+        <v>9999</v>
+      </c>
+      <c r="AMK11" s="1"/>
+      <c r="AMM11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="11" t="n">
-        <v>9999</v>
-      </c>
-      <c r="AMM11" s="0"/>
-      <c r="AMN11" s="1"/>
-      <c r="AMO11" s="1"/>
-      <c r="XFD11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="3" t="s">
+      <c r="M12" s="10" t="n">
+        <v>1111</v>
+      </c>
+      <c r="AMK12" s="1"/>
+      <c r="AMM12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="K13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="L13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMK13" s="1"/>
+      <c r="AMM13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="O12" s="11" t="n">
-        <v>1111</v>
-      </c>
-      <c r="AMM12" s="0"/>
-      <c r="AMN12" s="1"/>
-      <c r="AMO12" s="1"/>
-      <c r="XFD12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="H14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AMM13" s="0"/>
-      <c r="AMN13" s="1"/>
-      <c r="AMO13" s="1"/>
-      <c r="XFD13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O14" s="1" t="n">
+      <c r="M14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AMM14" s="0"/>
-      <c r="AMN14" s="1"/>
-      <c r="AMO14" s="1"/>
-      <c r="XFD14" s="0"/>
+      <c r="AMK14" s="1"/>
+      <c r="AMM14" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
SSDM-13256: Added missing column for sample.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t xml:space="preserve">SAMPLE</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">DEFAULT</t>
   </si>
   <si>
+    <t xml:space="preserve">PermId</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identifier</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">200001010000000-0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">/DEFAULT/DEFAULT/DEFAULT</t>
   </si>
   <si>
@@ -92,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Number of Boxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200001010000000-0001</t>
   </si>
   <si>
     <t xml:space="preserve">/ELN_SETTINGS/STORAGES/BENCH</t>
@@ -116,6 +125,9 @@
     <t xml:space="preserve">Bench</t>
   </si>
   <si>
+    <t xml:space="preserve">200001010000000-0002</t>
+  </si>
+  <si>
     <t xml:space="preserve">/ELN_SETTINGS/STORAGES/DEFAULT_STORAGE</t>
   </si>
   <si>
@@ -123,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Default Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200001010000000-0004</t>
   </si>
   <si>
     <t xml:space="preserve">/ELN_SETTINGS/STORAGES/CHILD_1</t>
@@ -136,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">Child 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200001010000000-0005</t>
   </si>
   <si>
     <t xml:space="preserve">/ELN_SETTINGS/STORAGES/CHILD_2</t>
@@ -342,15 +360,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMM14"/>
+  <dimension ref="A1:XFC14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.5"/>
@@ -362,8 +380,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1026" min="1026" style="1" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,7 +412,7 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -403,13 +421,13 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -421,50 +439,58 @@
       <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="9"/>
+      <c r="M4" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
-      <c r="AMK4" s="1"/>
+      <c r="Q4" s="9"/>
       <c r="AMM4" s="1"/>
+      <c r="AMN4" s="1"/>
+      <c r="XFC4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
+      <c r="A5" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AMK5" s="1"/>
+      <c r="L5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="AMM5" s="1"/>
+      <c r="AMN5" s="1"/>
+      <c r="XFC5" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -484,7 +510,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -495,7 +521,7 @@
       <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -504,13 +530,13 @@
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -522,178 +548,198 @@
       <c r="K10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
-      <c r="AMK10" s="1"/>
+      <c r="Q10" s="9"/>
       <c r="AMM10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>24</v>
+      <c r="AMN10" s="1"/>
+      <c r="XFC10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="10" t="n">
+        <v>9999</v>
+      </c>
+      <c r="AMM11" s="1"/>
+      <c r="AMN11" s="1"/>
+      <c r="XFC11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="J12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="K12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="10" t="n">
+        <v>1111</v>
+      </c>
+      <c r="AMM12" s="1"/>
+      <c r="AMN12" s="1"/>
+      <c r="XFC12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="10" t="n">
-        <v>9999</v>
-      </c>
-      <c r="AMK11" s="1"/>
-      <c r="AMM11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="G13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMM13" s="1"/>
+      <c r="AMN13" s="1"/>
+      <c r="XFC13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="J14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="10" t="n">
-        <v>1111</v>
-      </c>
-      <c r="AMK12" s="1"/>
-      <c r="AMM12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AMK13" s="1"/>
-      <c r="AMM13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="1" t="n">
+      <c r="K14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AMK14" s="1"/>
       <c r="AMM14" s="1"/>
+      <c r="AMN14" s="1"/>
+      <c r="XFC14" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>